<commit_message>
Add AI picklist recommendations to mapping Excel files
Updated BBF_Final_Value column in Picklist_Mapping sheets with:
- 76 AI-recommended picklist value mappings
- 11 items marked BUSINESS_DECISION_REQUIRED

Ready for business owner review and sign-off.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/day-two/mappings/ES_Account_to_BBF_Account_mapping.xlsx
+++ b/day-two/mappings/ES_Account_to_BBF_Account_mapping.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjero\Documents\repos\python-repo\python_scripts\ES-to-BBF-migration\day-two\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0685CF28-B435-46BB-AD84-5455C77F957B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7D8CD6-5547-4DE4-98C4-E0707CA67185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2895" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2895" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Field_Mapping" sheetId="1" r:id="rId1"/>
     <sheet name="Picklist_Mapping" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Field_Mapping!$A$1:$J$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Picklist_Mapping!$A$1:$H$103</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1876,8 +1880,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2197,21 +2201,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection sqref="A1:J151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:J151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="55.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6520,6 +6525,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J151" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6528,8 +6534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H103" sqref="A1:H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6537,10 +6544,10 @@
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="72.5546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="72.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="47.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8703,6 +8710,7 @@
       <c r="H103" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H103" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>